<commit_message>
before adding scene switch
</commit_message>
<xml_diff>
--- a/Dev IV Project Rubric.xlsx
+++ b/Dev IV Project Rubric.xlsx
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="100">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -965,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
@@ -1110,7 +1110,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1188,7 +1188,7 @@
       <c r="K6" s="5"/>
       <c r="L6" s="15">
         <f>IF(L4 &gt; 54, SUM(-54,L4),0)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -1316,11 +1316,11 @@
       </c>
       <c r="I10" s="19">
         <f>IF(H10+I4 - 18 &gt; 0, H10+I4 - 18, 0)</f>
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J10" s="19">
         <f>IF(I10+J4 - 18 &gt; 0, I10+J4 - 18, 0)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
@@ -2238,11 +2238,15 @@
       <c r="D49" s="5">
         <v>4</v>
       </c>
-      <c r="E49" s="2"/>
-      <c r="F49" s="3"/>
+      <c r="E49" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="G49" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H49" s="5"/>
       <c r="I49" s="5"/>
@@ -3144,7 +3148,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>